<commit_message>
Read files from actual path in excel finder
</commit_message>
<xml_diff>
--- a/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/WrongTemplateOneCamera-Channel1.xlsx
+++ b/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/WrongTemplateOneCamera-Channel1.xlsx
@@ -31,10 +31,10 @@
     <t xml:space="preserve">Pol0_45_90_135</t>
   </si>
   <si>
-    <t xml:space="preserve">Img1_C1.tif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Img2_C1.tif</t>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/OneCamera/Img1_C1.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/masoud/Documents/four-polar/fourPolar-io/src/test/resources/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/OneCamera/Img2_C1.tif</t>
   </si>
 </sst>
 </file>
@@ -135,13 +135,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
   </cols>
@@ -168,21 +168,21 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>